<commit_message>
Adding monster groups - continuing
</commit_message>
<xml_diff>
--- a/descent/src/descent-bdd.xlsx
+++ b/descent/src/descent-bdd.xlsx
@@ -4657,77 +4657,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="125">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="115">
     <dxf>
       <fill>
         <patternFill>
@@ -5811,8 +5741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK959"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A904" workbookViewId="0">
-      <selection activeCell="B927" sqref="B927"/>
+    <sheetView tabSelected="1" topLeftCell="B898" workbookViewId="0">
+      <selection activeCell="C931" sqref="C931"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32808,7 +32738,7 @@
         <v>75</v>
       </c>
       <c r="D807" t="str">
-        <f t="shared" ref="D807:D838" si="109">LOWER(REPLACE(A$742,SEARCH("_",A$742),1,""))&amp;"."&amp;LOWER(K807)&amp;"."&amp;LOWER(C807)</f>
+        <f t="shared" ref="D807:D814" si="109">LOWER(REPLACE(A$742,SEARCH("_",A$742),1,""))&amp;"."&amp;LOWER(K807)&amp;"."&amp;LOWER(C807)</f>
         <v>monstergroup.kobold.botw</v>
       </c>
       <c r="E807" t="s">
@@ -41075,7 +41005,7 @@
         <v/>
       </c>
       <c r="AE939" t="str">
-        <f t="shared" ref="AE927:AE958" si="145">IF(M939="","","insert into "&amp;A$891&amp;" ("&amp;B$891&amp;", "&amp;C$891&amp;", "&amp;D$891&amp;", "&amp;E$891&amp;", "&amp;F$891&amp;", "&amp;G$891&amp;", "&amp;H$891&amp;")
+        <f t="shared" ref="AE939:AE958" si="145">IF(M939="","","insert into "&amp;A$891&amp;" ("&amp;B$891&amp;", "&amp;C$891&amp;", "&amp;D$891&amp;", "&amp;E$891&amp;", "&amp;F$891&amp;", "&amp;G$891&amp;", "&amp;H$891&amp;")
 values ('"&amp;B939&amp;"', '"&amp;C939&amp;"', '"&amp;D939&amp;"', '"&amp;E939&amp;"', '"&amp;M939&amp;"', "&amp;IF(N939="","null",N939)&amp;", "&amp;IF(O939="","null",N939)&amp;");")</f>
         <v/>
       </c>
@@ -42469,421 +42399,421 @@
     <sortCondition ref="B178"/>
   </sortState>
   <conditionalFormatting sqref="B197:B198 B200:B218 B233:B258 R288 B287:B290">
-    <cfRule type="expression" dxfId="124" priority="144">
+    <cfRule type="expression" dxfId="114" priority="144">
       <formula>$H197="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="145">
+    <cfRule type="expression" dxfId="113" priority="145">
       <formula>$H197="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="146">
+    <cfRule type="expression" dxfId="112" priority="146">
       <formula>$H197="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="147">
+    <cfRule type="expression" dxfId="111" priority="147">
       <formula>$H197="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R197:R198">
-    <cfRule type="expression" dxfId="120" priority="140">
+    <cfRule type="expression" dxfId="110" priority="140">
       <formula>$H197="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="141">
+    <cfRule type="expression" dxfId="109" priority="141">
       <formula>$H197="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="142">
+    <cfRule type="expression" dxfId="108" priority="142">
       <formula>$H197="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="143">
+    <cfRule type="expression" dxfId="107" priority="143">
       <formula>$H197="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B199">
-    <cfRule type="expression" dxfId="116" priority="136">
+    <cfRule type="expression" dxfId="106" priority="136">
       <formula>$H199="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="137">
+    <cfRule type="expression" dxfId="105" priority="137">
       <formula>$H199="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="138">
+    <cfRule type="expression" dxfId="104" priority="138">
       <formula>$H199="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="139">
+    <cfRule type="expression" dxfId="103" priority="139">
       <formula>$H199="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R216">
-    <cfRule type="expression" dxfId="112" priority="132">
+    <cfRule type="expression" dxfId="102" priority="132">
       <formula>$H216="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="133">
+    <cfRule type="expression" dxfId="101" priority="133">
       <formula>$H216="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="134">
+    <cfRule type="expression" dxfId="100" priority="134">
       <formula>$H216="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="135">
+    <cfRule type="expression" dxfId="99" priority="135">
       <formula>$H216="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B229:B232">
-    <cfRule type="expression" dxfId="108" priority="128">
+    <cfRule type="expression" dxfId="98" priority="128">
       <formula>$H229="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="129">
+    <cfRule type="expression" dxfId="97" priority="129">
       <formula>$H229="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="130">
+    <cfRule type="expression" dxfId="96" priority="130">
       <formula>$H229="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="131">
+    <cfRule type="expression" dxfId="95" priority="131">
       <formula>$H229="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B223:B228">
-    <cfRule type="expression" dxfId="104" priority="124">
+    <cfRule type="expression" dxfId="94" priority="124">
       <formula>$H223="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="125">
+    <cfRule type="expression" dxfId="93" priority="125">
       <formula>$H223="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="126">
+    <cfRule type="expression" dxfId="92" priority="126">
       <formula>$H223="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="127">
+    <cfRule type="expression" dxfId="91" priority="127">
       <formula>$H223="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B219:B222">
-    <cfRule type="expression" dxfId="100" priority="120">
+    <cfRule type="expression" dxfId="90" priority="120">
       <formula>$H219="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="121">
+    <cfRule type="expression" dxfId="89" priority="121">
       <formula>$H219="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="122">
+    <cfRule type="expression" dxfId="88" priority="122">
       <formula>$H219="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="123">
+    <cfRule type="expression" dxfId="87" priority="123">
       <formula>$H219="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R223:R224">
-    <cfRule type="expression" dxfId="96" priority="116">
+    <cfRule type="expression" dxfId="86" priority="116">
       <formula>$H223="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="117">
+    <cfRule type="expression" dxfId="85" priority="117">
       <formula>$H223="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="118">
+    <cfRule type="expression" dxfId="84" priority="118">
       <formula>$H223="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="119">
+    <cfRule type="expression" dxfId="83" priority="119">
       <formula>$H223="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R222">
-    <cfRule type="expression" dxfId="92" priority="112">
+    <cfRule type="expression" dxfId="82" priority="112">
       <formula>$H222="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="113">
+    <cfRule type="expression" dxfId="81" priority="113">
       <formula>$H222="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="114">
+    <cfRule type="expression" dxfId="80" priority="114">
       <formula>$H222="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="115">
+    <cfRule type="expression" dxfId="79" priority="115">
       <formula>$H222="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R229:R230">
-    <cfRule type="expression" dxfId="88" priority="108">
+    <cfRule type="expression" dxfId="78" priority="108">
       <formula>$H229="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="109">
+    <cfRule type="expression" dxfId="77" priority="109">
       <formula>$H229="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="110">
+    <cfRule type="expression" dxfId="76" priority="110">
       <formula>$H229="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="111">
+    <cfRule type="expression" dxfId="75" priority="111">
       <formula>$H229="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R228">
-    <cfRule type="expression" dxfId="84" priority="104">
+    <cfRule type="expression" dxfId="74" priority="104">
       <formula>$H228="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="105">
+    <cfRule type="expression" dxfId="73" priority="105">
       <formula>$H228="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="106">
+    <cfRule type="expression" dxfId="72" priority="106">
       <formula>$H228="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="107">
+    <cfRule type="expression" dxfId="71" priority="107">
       <formula>$H228="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R233:R235">
-    <cfRule type="expression" dxfId="80" priority="100">
+    <cfRule type="expression" dxfId="70" priority="100">
       <formula>$H233="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="101">
+    <cfRule type="expression" dxfId="69" priority="101">
       <formula>$H233="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="102">
+    <cfRule type="expression" dxfId="68" priority="102">
       <formula>$H233="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="103">
+    <cfRule type="expression" dxfId="67" priority="103">
       <formula>$H233="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R232">
-    <cfRule type="expression" dxfId="76" priority="96">
+    <cfRule type="expression" dxfId="66" priority="96">
       <formula>$H232="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="97">
+    <cfRule type="expression" dxfId="65" priority="97">
       <formula>$H232="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="98">
+    <cfRule type="expression" dxfId="64" priority="98">
       <formula>$H232="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="99">
+    <cfRule type="expression" dxfId="63" priority="99">
       <formula>$H232="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B259:B286">
-    <cfRule type="expression" dxfId="72" priority="92">
+    <cfRule type="expression" dxfId="62" priority="92">
       <formula>$H259="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="93">
+    <cfRule type="expression" dxfId="61" priority="93">
       <formula>$H259="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="94">
+    <cfRule type="expression" dxfId="60" priority="94">
       <formula>$H259="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="95">
+    <cfRule type="expression" dxfId="59" priority="95">
       <formula>$H259="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R263:R270">
-    <cfRule type="expression" dxfId="68" priority="88">
+    <cfRule type="expression" dxfId="58" priority="88">
       <formula>$H263="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="89">
+    <cfRule type="expression" dxfId="57" priority="89">
       <formula>$H263="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="90">
+    <cfRule type="expression" dxfId="56" priority="90">
       <formula>$H263="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="91">
+    <cfRule type="expression" dxfId="55" priority="91">
       <formula>$H263="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R271">
-    <cfRule type="expression" dxfId="64" priority="84">
+    <cfRule type="expression" dxfId="54" priority="84">
       <formula>$H271="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="85">
+    <cfRule type="expression" dxfId="53" priority="85">
       <formula>$H271="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="86">
+    <cfRule type="expression" dxfId="52" priority="86">
       <formula>$H271="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="87">
+    <cfRule type="expression" dxfId="51" priority="87">
       <formula>$H271="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R274:R276">
-    <cfRule type="expression" dxfId="60" priority="80">
+    <cfRule type="expression" dxfId="50" priority="80">
       <formula>$H274="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="81">
+    <cfRule type="expression" dxfId="49" priority="81">
       <formula>$H274="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="82">
+    <cfRule type="expression" dxfId="48" priority="82">
       <formula>$H274="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="83">
+    <cfRule type="expression" dxfId="47" priority="83">
       <formula>$H274="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R272">
-    <cfRule type="expression" dxfId="56" priority="76">
+    <cfRule type="expression" dxfId="46" priority="76">
       <formula>$H272="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="77">
+    <cfRule type="expression" dxfId="45" priority="77">
       <formula>$H272="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="78">
+    <cfRule type="expression" dxfId="44" priority="78">
       <formula>$H272="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="79">
+    <cfRule type="expression" dxfId="43" priority="79">
       <formula>$H272="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R282">
-    <cfRule type="expression" dxfId="52" priority="72">
+    <cfRule type="expression" dxfId="42" priority="72">
       <formula>$H282="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="73">
+    <cfRule type="expression" dxfId="41" priority="73">
       <formula>$H282="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="74">
+    <cfRule type="expression" dxfId="40" priority="74">
       <formula>$H282="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="75">
+    <cfRule type="expression" dxfId="39" priority="75">
       <formula>$H282="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R284:R286">
-    <cfRule type="expression" dxfId="48" priority="68">
+    <cfRule type="expression" dxfId="38" priority="68">
       <formula>$H284="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="69">
+    <cfRule type="expression" dxfId="37" priority="69">
       <formula>$H284="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="70">
+    <cfRule type="expression" dxfId="36" priority="70">
       <formula>$H284="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="71">
+    <cfRule type="expression" dxfId="35" priority="71">
       <formula>$H284="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B291">
-    <cfRule type="expression" dxfId="44" priority="40">
+    <cfRule type="expression" dxfId="34" priority="40">
       <formula>$H291="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="41">
+    <cfRule type="expression" dxfId="33" priority="41">
       <formula>$H291="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="42">
+    <cfRule type="expression" dxfId="32" priority="42">
       <formula>$H291="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="43">
+    <cfRule type="expression" dxfId="31" priority="43">
       <formula>$H291="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B292">
-    <cfRule type="expression" dxfId="40" priority="36">
+    <cfRule type="expression" dxfId="30" priority="36">
       <formula>$H292="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="37">
+    <cfRule type="expression" dxfId="29" priority="37">
       <formula>$H292="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="38">
+    <cfRule type="expression" dxfId="28" priority="38">
       <formula>$H292="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="27" priority="39">
       <formula>$H292="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B293">
-    <cfRule type="expression" dxfId="36" priority="32">
+    <cfRule type="expression" dxfId="26" priority="32">
       <formula>$H293="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="33">
+    <cfRule type="expression" dxfId="25" priority="33">
       <formula>$H293="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="34">
+    <cfRule type="expression" dxfId="24" priority="34">
       <formula>$H293="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="35">
+    <cfRule type="expression" dxfId="23" priority="35">
       <formula>$H293="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R293">
-    <cfRule type="expression" dxfId="32" priority="28">
+    <cfRule type="expression" dxfId="22" priority="28">
       <formula>$H293="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="29">
+    <cfRule type="expression" dxfId="21" priority="29">
       <formula>$H293="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="30">
+    <cfRule type="expression" dxfId="20" priority="30">
       <formula>$H293="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="31">
+    <cfRule type="expression" dxfId="19" priority="31">
       <formula>$H293="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B294">
-    <cfRule type="expression" dxfId="28" priority="24">
+    <cfRule type="expression" dxfId="18" priority="24">
       <formula>$H294="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="25">
+    <cfRule type="expression" dxfId="17" priority="25">
       <formula>$H294="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="26">
+    <cfRule type="expression" dxfId="16" priority="26">
       <formula>$H294="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="15" priority="27">
       <formula>$H294="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R294">
-    <cfRule type="expression" dxfId="24" priority="20">
+    <cfRule type="expression" dxfId="14" priority="20">
       <formula>$H294="Eclaireur"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="21">
+    <cfRule type="expression" dxfId="13" priority="21">
       <formula>$H294="Mage"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="22">
+    <cfRule type="expression" dxfId="12" priority="22">
       <formula>$H294="Guerrier"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="23">
+    <cfRule type="expression" dxfId="11" priority="23">
       <formula>$H294="Soigneur"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A895:C895 F895:XFD895 Z896:AA958 AI896:AK918 AE896:AE938">
-    <cfRule type="expression" dxfId="5" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>$D895="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E895">
-    <cfRule type="expression" dxfId="20" priority="12">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>$D895="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A896:C957 AL896:XFD918 AB939:AH957 AL923:XFD957 F896:Y957 AB896:AD938 AF923:AH938 AF896:AH918 AF919:XFD922">
-    <cfRule type="expression" dxfId="19" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>$D896="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A895:AK895 Z896:AA958 AI896:AK918 AE896:AE938">
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>$E895="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E896:E957">
-    <cfRule type="expression" dxfId="18" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$D896="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB939:AH957 A896:Y957 AB896:AD938 AF923:AH938 AF896:AH918 AF919:AK922">
-    <cfRule type="expression" dxfId="17" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$E896="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A958:C958 F958:Y958 AB958:AH958 AL958:XFD958">
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$D958="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E958">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$D958="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A958:Y958 AB958:AH958">
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$E958="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI923:AK958">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$D923="Master"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI923:AK958">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E923="Master"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>